<commit_message>
[feature/ResolveReport] email service added
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Core value</t>
   </si>
@@ -56,37 +56,28 @@
     <t>new desc 1</t>
   </si>
   <si>
+    <t>Great teamwork!</t>
+  </si>
+  <si>
+    <t>Chetan</t>
+  </si>
+  <si>
+    <t>Satpute</t>
+  </si>
+  <si>
+    <t>Software Engineer</t>
+  </si>
+  <si>
+    <t>Ajinkya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karanjikar  </t>
+  </si>
+  <si>
+    <t>Technical Lead</t>
+  </si>
+  <si>
     <t>Great teamwork aditya!</t>
-  </si>
-  <si>
-    <t>Chetan</t>
-  </si>
-  <si>
-    <t>Satpute</t>
-  </si>
-  <si>
-    <t>Software Engineer</t>
-  </si>
-  <si>
-    <t>Amar</t>
-  </si>
-  <si>
-    <t>Jadhav</t>
-  </si>
-  <si>
-    <t>Senior Software Engineer</t>
-  </si>
-  <si>
-    <t>Great teamwork!</t>
-  </si>
-  <si>
-    <t>Ajinkya</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Karanjikar  </t>
-  </si>
-  <si>
-    <t>Technical Lead</t>
   </si>
   <si>
     <t>Aditya</t>
@@ -508,13 +499,13 @@
         <v>22</v>
       </c>
       <c r="I3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
@@ -537,53 +528,18 @@
         <v>16</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="I4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
       <c r="K4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated by for grades and badges
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Core value</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>Trainee</t>
+  </si>
+  <si>
+    <t>Great teamwork dskafkdfgkjahda a dhsfkjadhkfha hdkjfhakdhfkg sadhfkahdsjkfhakj aksjdhfkjahdkjfhakjsd akdshfkjahdfk</t>
   </si>
   <si>
     <t>Great teamwork!</t>
@@ -505,22 +508,22 @@
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
         <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="I3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -537,25 +540,25 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="F4" t="s">
         <v>16</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="I4" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -575,28 +578,28 @@
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
         <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="H5" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="I5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
       <c r="K5">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -610,28 +613,28 @@
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F6" t="s">
         <v>16</v>
       </c>
       <c r="G6" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="H6" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="I6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="J6">
         <v>0</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
@@ -642,30 +645,65 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="F7" t="s">
         <v>16</v>
       </c>
       <c r="G7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
         <v>23</v>
       </c>
-      <c r="H7" t="s">
+      <c r="F8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" t="s">
         <v>24</v>
       </c>
-      <c r="I7" t="s">
+      <c r="H8" t="s">
         <v>25</v>
       </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
+      <c r="I8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[feature/ResolveReport] mail template fixes
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -707,6 +707,41 @@
         <v>0</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>